<commit_message>
Added OSA01Study testcases Sofia_OSA01_46to58andTC44
</commit_message>
<xml_diff>
--- a/InputFiles/TC44_Canine_Study_MGT01_SampleSite_MammaryGland.xlsx
+++ b/InputFiles/TC44_Canine_Study_MGT01_SampleSite_MammaryGland.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davids3\newclone\ICDC All tab fix\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E133D8-EFEB-4B69-A04B-02A022DEC3E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F037D9C-9C05-4ABB-B0DF-7743B6AF7A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
   <si>
     <t>WebExcel</t>
   </si>
@@ -58,62 +58,6 @@
   </si>
   <si>
     <t>StudyFilesTab</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MATCH (p:program)&lt;--(s:study)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis), (c)&lt;--(r:registration)
-WHERE s.clinical_study_designation IN ['MGT01'] and diag.primary_disease_site in['Mammary Gland']
-OPTIONAL MATCH (cf:file)-[*]-&gt;(c)
-OPTIONAL MATCH (samp:sample)--&gt;(c)
-OPTIONAL MATCH (sf:file)--&gt;(s)
-RETURN
-	count(distinct p) AS Programs,
-    count(distinct s) AS Studies,
-    count(distinct c) AS Cases,
-    count(distinct samp) AS Samples,
-    count(distinct cf) AS `Case Files`,
-    count(distinct sf) AS `Study Files`
-    </t>
-  </si>
-  <si>
-    <t>TC05_Canine_Study_MGT01_PrimaryDiseaseSite_MammaryGland_Neo4jData.xlsx</t>
-  </si>
-  <si>
-    <t>TC05_Canine_Study_MGT01_PrimaryDiseaseSite_MammaryGland_WebData.xlsx</t>
-  </si>
-  <si>
-    <t>MATCH (f:file)--&gt;(parent)
-WITH DISTINCT f, parent
-MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
-MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
-MATCH (r:registration)--&gt;(c)
-WHERE s.clinical_study_designation IN ['MGT01'] and diag.primary_disease_site in['Mammary Gland']
-OPTIONAL MATCH (f)-[*]-&gt;(samp:sample)
-WITH
-        DISTINCT f, parent, c, demo, diag, s, samp,
-        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
-        toInteger(floor(log(f.file_size)/log(1024))) as i,
-        2 as precision
-WITH
-        f, parent, c, demo, diag, s, samp,
-        f.file_size /(1024^i) AS value,
-        10^precision AS factor,
-        units[i] as unit
-WITH
-        f, parent, c, demo, diag, s, samp, unit,
-        round(factor * value)/factor AS size
-RETURN
-        coalesce(f.file_name, '') AS `File Name`,
-        coalesce(f.file_format, '') AS `Format`,
-        coalesce(f.file_type, '') AS `File Type`,
-        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
-        coalesce(labels(parent)[0], '') AS `Association`,
-        coalesce(f.file_description, '') AS `Description`,
-        coalesce(samp.sample_id, '') AS `Sample ID`,
-        coalesce(c.case_id, '') AS `Case ID`,
-        coalesce(demo.breed,'') AS Breed ,
-        coalesce(diag.disease_term,'') AS Diagnosis
-        order by f.file_name asc
-        limit 100</t>
   </si>
   <si>
     <t xml:space="preserve">MATCH (p:program)&lt;--(s:study)&lt;--(c:case)&lt;--(demo:demographic), (c)&lt;--(diag:diagnosis), (c)&lt;--(r:registration)
@@ -199,6 +143,48 @@
   coalesce(s.clinical_study_designation,'') AS `Study Code`
   order by 'File Name' asc
   limit 100</t>
+  </si>
+  <si>
+    <t>TC44_Canine_Study_MGT01_SampleSite_MammaryGland_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC44_Canine_Study_MGT01_SampleSite_MammaryGland_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+MATCH (s:study)&lt;-[*]-(c)&lt;--(diag:diagnosis)
+MATCH (r:registration)--&gt;(c)
+MATCH (f)-[*]-&gt;(samp:sample)
+WHERE s.clinical_study_designation IN ['MGT01'] and samp.sample_site in['Mammary Gland']
+OPTIONAL MATCH (f)-[*]-&gt;(samp:sample)
+WITH
+        DISTINCT f, parent, c, demo, diag, s, samp,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, parent, c, demo, diag, s, samp,
+        f.file_size /(1024^i) AS value,
+        10^precision AS factor,
+        units[i] as unit
+WITH
+        f, parent, c, demo, diag, s, samp, unit,
+        round(factor * value)/factor AS size
+RETURN
+        coalesce(f.file_name, '') AS `File Name`,
+        coalesce(f.file_format, '') AS `Format`,
+        coalesce(f.file_type, '') AS `File Type`,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+        coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`,
+        coalesce(samp.sample_id, '') AS `Sample ID`,
+        coalesce(c.case_id, '') AS `Case ID`,
+        coalesce(demo.breed,'') AS Breed ,
+        coalesce(diag.disease_term,'') AS Diagnosis
+        order by f.file_name asc
+        limit 100</t>
   </si>
 </sst>
 </file>
@@ -579,7 +565,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>
@@ -616,16 +602,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.3">
@@ -633,16 +619,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.3">
@@ -650,16 +636,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.3">
@@ -667,16 +653,16 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>